<commit_message>
Finally figured out slideshow
</commit_message>
<xml_diff>
--- a/Wireframing.xlsx
+++ b/Wireframing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DFayinke\bootcamp\projects\Week2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DFayinke\bootcamp\projects\estate-agent\estate-agent-webpage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4314F7B6-AC23-495E-AF56-464C129EDEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8EFA0A-E3A3-4FF7-98B8-E722A2FFA1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CAB0ADA6-9F79-4C1A-81C0-BDA4A0989649}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Home</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Rentals</t>
   </si>
   <si>
-    <t>Why choose me?</t>
-  </si>
-  <si>
     <t>See Properties</t>
   </si>
   <si>
@@ -84,6 +81,12 @@
   </si>
   <si>
     <t xml:space="preserve">copyright </t>
+  </si>
+  <si>
+    <t>Letting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testimonials </t>
   </si>
 </sst>
 </file>
@@ -166,28 +169,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,54 +413,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -514,6 +461,22 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -562,6 +525,22 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -576,6 +555,22 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -735,40 +730,40 @@
     <tableColumn id="8" xr3:uid="{1633FAA3-B2BA-4B05-9719-317FD6E5B5FD}" name="Column8" dataDxfId="47"/>
     <tableColumn id="9" xr3:uid="{2B3AEF8A-308B-4E37-B7F1-F237C99F74E1}" name="Column9" dataDxfId="46"/>
     <tableColumn id="10" xr3:uid="{5D637629-5639-4296-931B-9BBAE26B7BAF}" name="Column10" dataDxfId="45"/>
-    <tableColumn id="11" xr3:uid="{948A4F12-770C-40B2-A1F7-3044B1145FEF}" name="Column11" headerRowDxfId="22" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{948A4F12-770C-40B2-A1F7-3044B1145FEF}" name="Column11" headerRowDxfId="44" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99D860EF-1252-42DE-A67E-D1BE0AD8565C}" name="Table24" displayName="Table24" ref="B13:D20" headerRowCount="0" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99D860EF-1252-42DE-A67E-D1BE0AD8565C}" name="Table24" displayName="Table24" ref="B13:D20" headerRowCount="0" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" tableBorderDxfId="40">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C9E5DDC2-33A3-45CF-89D6-CE63E9AB4A64}" name="Column1" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{FB100A8C-F93A-46E1-AC3B-59EE3D701F79}" name="Column2" dataDxfId="40"/>
-    <tableColumn id="11" xr3:uid="{157FCE81-DC8E-4011-8626-8D0198603AEA}" name="Column3" headerRowDxfId="28" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{C9E5DDC2-33A3-45CF-89D6-CE63E9AB4A64}" name="Column1" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{FB100A8C-F93A-46E1-AC3B-59EE3D701F79}" name="Column2" dataDxfId="38"/>
+    <tableColumn id="11" xr3:uid="{157FCE81-DC8E-4011-8626-8D0198603AEA}" name="Column3" headerRowDxfId="37" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3DF652F0-C805-4329-9844-B83DC1002FE8}" name="Table245" displayName="Table245" ref="F13:H20" headerRowCount="0" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3DF652F0-C805-4329-9844-B83DC1002FE8}" name="Table245" displayName="Table245" ref="F13:H20" headerRowCount="0" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2AD9CB24-57AA-4B32-BE70-0614E870D5D9}" name="Column1" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{539A21D7-B087-40A6-B119-BEB94A78004E}" name="Column2" dataDxfId="35"/>
-    <tableColumn id="11" xr3:uid="{7D19AF77-5268-4E30-BEDD-A95FD5776FE9}" name="Column3" headerRowDxfId="26" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{2AD9CB24-57AA-4B32-BE70-0614E870D5D9}" name="Column1" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{539A21D7-B087-40A6-B119-BEB94A78004E}" name="Column2" dataDxfId="31"/>
+    <tableColumn id="11" xr3:uid="{7D19AF77-5268-4E30-BEDD-A95FD5776FE9}" name="Column3" headerRowDxfId="30" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2DB4C3E1-24C6-4418-9343-D18A17C129B9}" name="Table246" displayName="Table246" ref="J13:L20" headerRowCount="0" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" tableBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2DB4C3E1-24C6-4418-9343-D18A17C129B9}" name="Table246" displayName="Table246" ref="J13:L20" headerRowCount="0" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{25B710FB-930A-4E29-B0CE-DC6F0D692D13}" name="Column1" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{0E3F0BA0-A023-4BE6-8BEF-ED24541DA57A}" name="Column2" dataDxfId="30"/>
-    <tableColumn id="11" xr3:uid="{B99DF2F7-18F8-4670-842C-317F5D7B18BD}" name="Column3" headerRowDxfId="24" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{25B710FB-930A-4E29-B0CE-DC6F0D692D13}" name="Column1" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{0E3F0BA0-A023-4BE6-8BEF-ED24541DA57A}" name="Column2" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{B99DF2F7-18F8-4670-842C-317F5D7B18BD}" name="Column3" headerRowDxfId="23" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -780,10 +775,10 @@
     <tableColumn id="1" xr3:uid="{2A913EEB-614A-43A9-B3D4-177E7AC40D4D}" name="Column1" dataDxfId="18"/>
     <tableColumn id="2" xr3:uid="{62EE61AB-AD5E-40FF-9490-F547AF3A0372}" name="Column2" dataDxfId="17"/>
     <tableColumn id="11" xr3:uid="{10D6575E-EB37-4989-B909-74AE4BE40A2F}" name="Column3" headerRowDxfId="16" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{55FB5466-2CD7-4E86-98D0-1CD34FA16236}" name="Column4" headerRowDxfId="13" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{30268B48-4AD1-4786-AF8A-ADE9EC3444CC}" name="Column5" headerRowDxfId="11" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{CAB22AD9-72CE-43E5-9F08-4EC0B464A85B}" name="Column6" headerRowDxfId="9" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{9183B597-C898-47D9-BE53-F411FD5834C4}" name="Column7" headerRowDxfId="7" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{55FB5466-2CD7-4E86-98D0-1CD34FA16236}" name="Column4" headerRowDxfId="14" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{30268B48-4AD1-4786-AF8A-ADE9EC3444CC}" name="Column5" headerRowDxfId="12" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{CAB22AD9-72CE-43E5-9F08-4EC0B464A85B}" name="Column6" headerRowDxfId="10" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{9183B597-C898-47D9-BE53-F411FD5834C4}" name="Column7" headerRowDxfId="8" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1117,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A58BCAA-C509-4D09-A3D0-E86580D18ADB}">
-  <dimension ref="B1:L34"/>
+  <dimension ref="C1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1130,18 +1125,18 @@
     <col min="11" max="11" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -1154,320 +1149,102 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:11" x14ac:dyDescent="0.35">
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5" t="s">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="4"/>
-      <c r="C14" s="6" t="s">
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="G13"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="6" t="s">
+      <c r="F14"/>
+      <c r="G14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="2"/>
-      <c r="C18" s="7" t="s">
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="F15"/>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="F16"/>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F17"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="F18"/>
+      <c r="G18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="K18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D19"/>
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D20"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L18" s="9"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="2"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B25" s="4"/>
-      <c r="C25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="2"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="5" t="s">
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="J27" t="s">
         <v>10</v>
       </c>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="2"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="2"/>
-      <c r="J27" s="4" t="s">
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="J28" t="s">
         <v>11</v>
       </c>
-      <c r="K27" s="10"/>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="2"/>
-      <c r="J28" s="4" t="s">
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="J29" t="s">
         <v>12</v>
       </c>
-      <c r="K28" s="10"/>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="2"/>
-      <c r="J29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K29" s="10"/>
-      <c r="L29" s="4"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D31"/>
     </row>
     <row r="34" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>